<commit_message>
JAVA github Code Release Version 1
</commit_message>
<xml_diff>
--- a/resource/file/数据库字段对应.xlsx
+++ b/resource/file/数据库字段对应.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86913\Documents\GitHub\cpManagement\resource\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674FB435-98FC-4A32-AE36-149BAE41EFFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66945C87-03D1-45B7-AB7A-DA80C441AFEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="309">
   <si>
     <t xml:space="preserve">委托书 </t>
   </si>
@@ -946,6 +946,39 @@
   </si>
   <si>
     <t>生成整备质量+100</t>
+  </si>
+  <si>
+    <t>达标车量编号</t>
+  </si>
+  <si>
+    <t>${DBCLBH}</t>
+  </si>
+  <si>
+    <t>国产进口</t>
+  </si>
+  <si>
+    <t>核定载质量</t>
+  </si>
+  <si>
+    <t>hdzzl</t>
+  </si>
+  <si>
+    <t>${hdzzl}</t>
+  </si>
+  <si>
+    <t>身份证号码</t>
+  </si>
+  <si>
+    <t>gcjk</t>
+  </si>
+  <si>
+    <t>sfzmhm</t>
+  </si>
+  <si>
+    <t>${sfzmhm}</t>
+  </si>
+  <si>
+    <t>${GCJK}</t>
   </si>
 </sst>
 </file>
@@ -1594,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H190"/>
+  <dimension ref="A2:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3779,6 +3812,51 @@
         <v>296</v>
       </c>
     </row>
+    <row r="191" spans="1:8" s="50" customFormat="1">
+      <c r="A191" s="49" t="s">
+        <v>298</v>
+      </c>
+      <c r="B191" s="49"/>
+      <c r="E191" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="F191" s="51"/>
+      <c r="G191" s="49"/>
+      <c r="H191" s="49"/>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="D192" t="s">
+        <v>305</v>
+      </c>
+      <c r="E192" s="50" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="D193" t="s">
+        <v>302</v>
+      </c>
+      <c r="E193" s="50" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D194" t="s">
+        <v>306</v>
+      </c>
+      <c r="E194" s="50" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>